<commit_message>
Updated API version to 2.5.0
</commit_message>
<xml_diff>
--- a/documents/Published/CylindricalGauge/CylindricalGaugeByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/CylindricalGauge/CylindricalGaugeByMAQSoftwareChecklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gitlab_Repos\documents\Published\CylindricalGauge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC74FFB0-FD5F-4688-9158-105C85B650F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{16A5F0D4-301B-4A8E-9F9A-CD7B785A2B97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CA504DF-EEC1-406B-8211-12A36D5258A3}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
   <si>
     <t>S no</t>
   </si>
@@ -285,6 +285,18 @@
   </si>
   <si>
     <t>Visual should be rendered properly.</t>
+  </si>
+  <si>
+    <t>Internet Explorer</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Desktop</t>
   </si>
 </sst>
 </file>
@@ -349,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -381,6 +393,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,6 +411,1595 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>409575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3000759</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3334158</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8B3F0BF-89B5-4362-BCC8-CC82059D36E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13230225" y="600075"/>
+          <a:ext cx="2753109" cy="2924583"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>552450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2562572</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3210296</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{857D405F-A3E4-44EC-85E1-B998ED5EEE58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12449175" y="742950"/>
+          <a:ext cx="2486372" cy="2657846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>904875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2866345</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D417FE41-268C-43E0-B4B0-954994E80345}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11991975" y="1095375"/>
+          <a:ext cx="2066925" cy="1961470"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2591131</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2886451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E474A03-4D1E-45B0-8533-AD7FD64E4E2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10896600" y="381000"/>
+          <a:ext cx="2372056" cy="2695951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2054189</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2009775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D3A76E2-95B1-4C4B-AA1B-4FFC2A9CE095}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13487400" y="4314825"/>
+          <a:ext cx="1958939" cy="1828800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2171700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2008199</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81313E4F-DF50-46EE-B728-D69F588D88E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15916275" y="4257675"/>
+          <a:ext cx="1914525" cy="1884374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2219325</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2036774</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51C67FEF-BFC3-4FEC-AC7B-B74BADEBE774}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10982325" y="4286250"/>
+          <a:ext cx="1914525" cy="1884374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2171700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1895543</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5775B4B2-02BE-47AE-8AB6-1F5B81C30EDF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18849975" y="4133851"/>
+          <a:ext cx="1771650" cy="1895542"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2133157</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2028826</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C822B24E-F6F5-4723-A17E-65BAA73E504A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13506450" y="6343651"/>
+          <a:ext cx="2018857" cy="1866900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2028826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2551430</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2647951</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB606C86-40D7-42D7-AF1C-7F67E4CE2401}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10810875" y="6162676"/>
+          <a:ext cx="2418080" cy="2667000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2371725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2463534</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE3249DB-E1D1-4109-A6A8-1C20D3F66FFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15659100" y="6181725"/>
+          <a:ext cx="2371725" cy="2463534"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2371725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2559827</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E11FFE1-9E50-4DD3-BC68-0567253997B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18449925" y="6181725"/>
+          <a:ext cx="2371725" cy="2559827"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2609851</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2428875</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2223559</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F02253D-2026-4C77-B849-6EE2AD9D0D26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18764250" y="8791576"/>
+          <a:ext cx="2114550" cy="2271183"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2628900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2476500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2268862</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25E6AA75-5C0C-4661-95A0-1428E62A328A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16068675" y="8810625"/>
+          <a:ext cx="2066925" cy="2297437"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2628901</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2228850</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2290376</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{726C6986-AD31-40A5-B5D8-B2384ED35539}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10801350" y="8810626"/>
+          <a:ext cx="2105025" cy="2318950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2216243</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2057400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6FBF4E4-DA09-4946-B943-747F1ED37F60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13392150" y="8839200"/>
+          <a:ext cx="2216243" cy="2057400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2257426</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2124075</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1848303</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A91B478-2359-4F15-A41C-BDDDB5466BED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18764251" y="11096626"/>
+          <a:ext cx="1809749" cy="1895927"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>323851</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2390775</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>899</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD5E3C52-03B0-4643-930D-E8C487C5BD27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15982951" y="11163300"/>
+          <a:ext cx="2066924" cy="2277374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2143125</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2150709</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF1DEC0E-037D-4F84-894E-E2B3C9484D8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13563601" y="11201400"/>
+          <a:ext cx="1971674" cy="2093559"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2495550</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2181034</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27CE3A33-28BC-4B26-A4C0-84823A6E535F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10906125" y="11172826"/>
+          <a:ext cx="2266950" cy="2152458"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2466975</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>31422</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB218737-19E5-4D8F-9717-EEC727B7D750}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18859500" y="13439775"/>
+          <a:ext cx="2057400" cy="2241222"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>447676</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2257426</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2097306</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8573C711-285E-4B59-8CDA-8DDE108AF5DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16106776" y="13525500"/>
+          <a:ext cx="1809750" cy="2011581"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2133600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2007500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92875EA7-7293-4A3C-A47F-3EB6C7A953A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11010900" y="13468351"/>
+          <a:ext cx="1800225" cy="1978924"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2286000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1971675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1969399</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECECFAE7-0C58-40C0-9FA1-42FF44D4300D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13563600" y="13430250"/>
+          <a:ext cx="1800225" cy="1978924"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2381250</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2218994</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70D31E79-2A2F-471C-8E3C-E3F316683B58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18840450" y="15725775"/>
+          <a:ext cx="1990725" cy="2142794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2371725</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>60419</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9136383-595D-4E63-8631-B5B1E57F0E5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10982325" y="15649576"/>
+          <a:ext cx="2066925" cy="2308318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2181225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>31843</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{814C1F25-66FB-4836-9DF0-F4D63C50A922}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13420725" y="15621000"/>
+          <a:ext cx="2066925" cy="2308318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2295525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>60418</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67B118CE-A4EF-49C5-B491-0ED9152525F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15887700" y="15649575"/>
+          <a:ext cx="2066925" cy="2308318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>361951</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2504327</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>2476912</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E61E4210-9CF9-40CD-B7B0-1B8B60B13CCA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18811876" y="18068924"/>
+          <a:ext cx="2142376" cy="2305463"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>361951</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2362201</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>2322167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E9B764A-599F-46C8-A932-4E974AD77CCE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11039476" y="17983200"/>
+          <a:ext cx="2000250" cy="2236442"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2117820</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>2381250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48DCBF7F-584D-4AEE-93D3-80B4A38ED051}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13601701" y="18145125"/>
+          <a:ext cx="1908269" cy="2133600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2190751</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>2424693</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D948BA4-7FDE-498E-9DC6-F845A084FB09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15868651" y="18107025"/>
+          <a:ext cx="1981200" cy="2215143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2276475</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1990525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EF7675D-896E-4965-8CE2-17FA8FD97A11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18907125" y="20526375"/>
+          <a:ext cx="1819275" cy="1933375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361951</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76481</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2095501</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2008334</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4A9CF0E-7279-42DB-9FE7-F87644477447}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16021051" y="20545706"/>
+          <a:ext cx="1733550" cy="1931853"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1907271</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2038350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CDCDF57-49B7-43B5-8AF8-D23087C39D37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13487401" y="20488276"/>
+          <a:ext cx="1812020" cy="2019299"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2162175</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1975119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE4D5EBF-9CF6-4954-BFF7-D952DACD496F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11144250" y="20554950"/>
+          <a:ext cx="1695450" cy="1889394"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -695,10 +2299,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF89ECC3-919A-4CE0-A09A-814B2A8DA1B6}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,10 +2312,14 @@
     <col min="3" max="3" width="37.7109375" style="8" customWidth="1"/>
     <col min="4" max="4" width="49.140625" style="8" customWidth="1"/>
     <col min="5" max="5" width="42.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="6" max="6" width="40.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="34" style="3" customWidth="1"/>
+    <col min="8" max="8" width="41.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="46.7109375" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -727,8 +2335,20 @@
       <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="310.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -745,7 +2365,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -762,7 +2382,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="7"/>
       <c r="D4" s="6" t="s">
         <v>51</v>
@@ -771,7 +2391,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="7"/>
       <c r="D5" s="6" t="s">
         <v>53</v>
@@ -780,7 +2400,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="7"/>
       <c r="D6" s="6" t="s">
         <v>44</v>
@@ -789,7 +2409,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -806,7 +2426,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="177" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -823,7 +2443,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="202.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -840,7 +2460,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -859,6 +2479,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -867,7 +2488,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,7 +2518,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -908,7 +2529,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -919,7 +2540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -952,7 +2573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -974,7 +2595,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -985,7 +2606,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -996,7 +2617,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1051,7 +2672,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1072,7 +2693,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1083,7 +2704,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1109,7 +2730,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>19</v>
       </c>
@@ -1120,7 +2741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20</v>
       </c>

</xml_diff>